<commit_message>
Working out rest of categorical tables
</commit_message>
<xml_diff>
--- a/Chapter_3_Figures.xlsx
+++ b/Chapter_3_Figures.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t xml:space="preserve">MODE2023</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">Vaginal birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unweighted_n</t>
   </si>
   <si>
     <t xml:space="preserve">AIAN</t>
@@ -481,13 +484,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>0.317566611821448</v>
+        <v>0.317230528327866</v>
       </c>
       <c r="C2" t="n">
-        <v>0.295456463904591</v>
+        <v>0.295133200068097</v>
       </c>
       <c r="D2" t="n">
-        <v>0.340531624785499</v>
+        <v>0.340183848916878</v>
       </c>
     </row>
     <row r="3">
@@ -495,13 +498,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.682433388178552</v>
+        <v>0.682769471672134</v>
       </c>
       <c r="C3" t="n">
-        <v>0.659468375214501</v>
+        <v>0.659816151083122</v>
       </c>
       <c r="D3" t="n">
-        <v>0.704543536095409</v>
+        <v>0.704866799931903</v>
       </c>
     </row>
   </sheetData>
@@ -549,70 +552,351 @@
       <c r="J1" t="s">
         <v>14</v>
       </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0288207660823145</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.366826161123008</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.00386123748115051</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.0173173675827501</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.0823091123745785</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.0476578048282393</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.384041503131194</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.00196166046849942</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
       <c r="J2" t="n">
-        <v>0.0672043875009834</v>
-      </c>
+        <v>0.00197947757518604</v>
+      </c>
+      <c r="K2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3" t="n">
+        <v>0.00385296910874353</v>
+      </c>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4" t="n">
+        <v>0.0171777680636307</v>
+      </c>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>15</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0287027759063095</v>
+      </c>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>25</v>
+      </c>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6" t="n">
+        <v>0.0477580996623627</v>
+      </c>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="n">
+        <v>35</v>
+      </c>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7" t="n">
+        <v>0.067094887786143</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="n">
+        <v>43</v>
+      </c>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8" t="n">
+        <v>0.0823547704495338</v>
+      </c>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="n">
+        <v>191</v>
+      </c>
+      <c r="C9"/>
+      <c r="D9" t="n">
+        <v>0.367082635169172</v>
+      </c>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="n">
+        <v>200</v>
+      </c>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10" t="n">
+        <v>0.383996616837657</v>
+      </c>
+      <c r="J10"/>
+      <c r="K10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="n">
-        <v>0.0232125337548346</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.350813536778905</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.00268312480141833</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.0116094382120037</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.0919206181152196</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.0546918937289626</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.373350389424773</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.00629035018056523</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.0854281151364933</v>
-      </c>
+      <c r="B11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11" t="n">
+        <v>0.00268385385482249</v>
+      </c>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="n">
+        <v>7</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12" t="n">
+        <v>0.00617164998937549</v>
+      </c>
+      <c r="K12"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="n">
+        <v>13</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13" t="n">
+        <v>0.0116588413874115</v>
+      </c>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="n">
+        <v>26</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0232951584971545</v>
+      </c>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="n">
+        <v>61</v>
+      </c>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15" t="n">
+        <v>0.0545216819632302</v>
+      </c>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="n">
+        <v>96</v>
+      </c>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16" t="n">
+        <v>0.085693408411084</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="n">
+        <v>103</v>
+      </c>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17" t="n">
+        <v>0.0918545852883654</v>
+      </c>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="n">
+        <v>393</v>
+      </c>
+      <c r="C18"/>
+      <c r="D18" t="n">
+        <v>0.350696883673852</v>
+      </c>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="n">
+        <v>419</v>
+      </c>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19" t="n">
+        <v>0.373423937070031</v>
+      </c>
+      <c r="J19"/>
+      <c r="K19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -633,7 +917,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>
@@ -646,6 +930,9 @@
       </c>
       <c r="F1" t="s">
         <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -653,40 +940,150 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>0.565228680555121</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.0134690981464368</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C2"/>
       <c r="D2" t="n">
-        <v>0.0344650831954583</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.369514491907749</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.0173226454302078</v>
-      </c>
+        <v>0.0133931610353742</v>
+      </c>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>9</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3" t="n">
+        <v>0.0170405777990429</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
+        <v>18</v>
+      </c>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4" t="n">
+        <v>0.0345416017665064</v>
+      </c>
+      <c r="F4"/>
+      <c r="G4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>193</v>
+      </c>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5" t="n">
+        <v>0.37036251915929</v>
+      </c>
+      <c r="G5"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>294</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.564662139498537</v>
+      </c>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="n">
-        <v>0.602136094113465</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.00981696808864679</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.0393228352899545</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.334427972477163</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.0142961300325847</v>
-      </c>
+      <c r="B7" t="n">
+        <v>11</v>
+      </c>
+      <c r="C7"/>
+      <c r="D7" t="n">
+        <v>0.0096772265166275</v>
+      </c>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="n">
+        <v>16</v>
+      </c>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8" t="n">
+        <v>0.0144398416956021</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="n">
+        <v>44</v>
+      </c>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9" t="n">
+        <v>0.0393677013113937</v>
+      </c>
+      <c r="F9"/>
+      <c r="G9"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="n">
+        <v>375</v>
+      </c>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10" t="n">
+        <v>0.334672892674186</v>
+      </c>
+      <c r="G10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="n">
+        <v>675</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.601842337804441</v>
+      </c>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -704,7 +1101,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -718,86 +1115,86 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>0.173886022552712</v>
+        <v>0.174184986825197</v>
       </c>
       <c r="C2" t="n">
-        <v>0.13372398465773</v>
+        <v>0.134016229488968</v>
       </c>
       <c r="D2" t="n">
-        <v>0.223005004554295</v>
+        <v>0.223289150556153</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0108030716823705</v>
+        <v>0.0108047363018289</v>
       </c>
       <c r="C3" t="n">
-        <v>0.00346379179593669</v>
+        <v>0.00347078628708757</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0331755348117452</v>
+        <v>0.0331206413743629</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" t="n">
-        <v>0.192660695065197</v>
+        <v>0.192490044523662</v>
       </c>
       <c r="C4" t="n">
-        <v>0.150404493327795</v>
+        <v>0.15031864236688</v>
       </c>
       <c r="D4" t="n">
-        <v>0.243387792903701</v>
+        <v>0.243107442802895</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" t="n">
-        <v>0.213052994614173</v>
+        <v>0.213428115682561</v>
       </c>
       <c r="C5" t="n">
-        <v>0.16885839374516</v>
+        <v>0.16923019232049</v>
       </c>
       <c r="D5" t="n">
-        <v>0.265124763512287</v>
+        <v>0.265480492188319</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" t="n">
-        <v>0.370739273265083</v>
+        <v>0.370200226457288</v>
       </c>
       <c r="C6" t="n">
-        <v>0.315887999021023</v>
+        <v>0.315464392104879</v>
       </c>
       <c r="D6" t="n">
-        <v>0.429140356550247</v>
+        <v>0.428488421885576</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0388579457693861</v>
+        <v>0.0388918902099839</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0215634468936572</v>
+        <v>0.0216023998566311</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0690443274672142</v>
+        <v>0.0690425507953225</v>
       </c>
     </row>
   </sheetData>
@@ -816,7 +1213,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -830,142 +1227,142 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0615780123850325</v>
+        <v>0.0617466200419983</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0359253744364647</v>
+        <v>0.036066472619278</v>
       </c>
       <c r="D2" t="n">
-        <v>0.103579992156073</v>
+        <v>0.103743701991065</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" t="n">
-        <v>0.512471252957583</v>
+        <v>0.512083276022754</v>
       </c>
       <c r="C3" t="n">
-        <v>0.44465270588808</v>
+        <v>0.444407027126909</v>
       </c>
       <c r="D3" t="n">
-        <v>0.579833724424863</v>
+        <v>0.579319408673184</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0189408236442159</v>
+        <v>0.0190949020269311</v>
       </c>
       <c r="C4" t="n">
-        <v>0.00706835718707399</v>
+        <v>0.00714212145958061</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0497557662094342</v>
+        <v>0.0500431478327114</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0234410402591145</v>
+        <v>0.0234024906805908</v>
       </c>
       <c r="C5" t="n">
-        <v>0.009717672794246</v>
+        <v>0.00971897983175979</v>
       </c>
       <c r="D5" t="n">
-        <v>0.055459284694198</v>
+        <v>0.055275886011655</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" t="n">
-        <v>0.128144150721643</v>
+        <v>0.128395682324831</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0890906962600912</v>
+        <v>0.0893448886190975</v>
       </c>
       <c r="D6" t="n">
-        <v>0.180916837110611</v>
+        <v>0.181120056608286</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0283459389182081</v>
+        <v>0.0281352702729767</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0127050600475863</v>
+        <v>0.0126293323462223</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0620321046600185</v>
+        <v>0.061493292968779</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B8" t="n">
-        <v>0.099335031683503</v>
+        <v>0.0995206098133455</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0654289237913471</v>
+        <v>0.0656116175324301</v>
       </c>
       <c r="D8" t="n">
-        <v>0.14802867861223</v>
+        <v>0.148175184220523</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0759606936358627</v>
+        <v>0.0755642333788086</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0468632190875981</v>
+        <v>0.0466598275930105</v>
       </c>
       <c r="D9" t="n">
-        <v>0.120834439405073</v>
+        <v>0.120118045319025</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0375196766213462</v>
+        <v>0.0376594805601157</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0187607241505598</v>
+        <v>0.0188582116040506</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0736283447960647</v>
+        <v>0.0737954028103382</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" t="n">
-        <v>0.0142633812534888</v>
+        <v>0.0143974368570601</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0045649952774538</v>
+        <v>0.00461912806097874</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0436623427369417</v>
+        <v>0.0439613919810137</v>
       </c>
     </row>
   </sheetData>
@@ -1001,13 +1398,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>0.317566611821448</v>
+        <v>0.317230528327866</v>
       </c>
       <c r="C2" t="n">
-        <v>0.295456463904591</v>
+        <v>0.295133200068097</v>
       </c>
       <c r="D2" t="n">
-        <v>0.340531624785499</v>
+        <v>0.340183848916878</v>
       </c>
     </row>
     <row r="3">
@@ -1015,13 +1412,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.682433388178552</v>
+        <v>0.682769471672134</v>
       </c>
       <c r="C3" t="n">
-        <v>0.659468375214501</v>
+        <v>0.659816151083122</v>
       </c>
       <c r="D3" t="n">
-        <v>0.704543536095409</v>
+        <v>0.704866799931903</v>
       </c>
     </row>
   </sheetData>
@@ -1040,7 +1437,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1054,156 +1451,156 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" t="n">
-        <v>0.00791253581117677</v>
+        <v>0.00793891752254143</v>
       </c>
       <c r="C2" t="n">
-        <v>0.00459689821191945</v>
+        <v>0.00461219332754814</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0135870236798715</v>
+        <v>0.0136323085049964</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0658505684906322</v>
+        <v>0.0658398285111455</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0548049367553515</v>
+        <v>0.0547954523290476</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0789364697835435</v>
+        <v>0.0789243938150372</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" t="n">
-        <v>0.00243382249023144</v>
+        <v>0.00245507944710004</v>
       </c>
       <c r="C4" t="n">
-        <v>0.000912629426638868</v>
+        <v>0.000920735986738353</v>
       </c>
       <c r="D4" t="n">
-        <v>0.00647414678669508</v>
+        <v>0.00652959044219068</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B5" t="n">
-        <v>0.003012082771419</v>
+        <v>0.00300891681128043</v>
       </c>
       <c r="C5" t="n">
-        <v>0.00125293003148791</v>
+        <v>0.00125157461090693</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0072232774895944</v>
+        <v>0.00721592447015689</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0164660263862675</v>
+        <v>0.0165081542422898</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0113102547449377</v>
+        <v>0.0113397944708772</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0239152030825681</v>
+        <v>0.0239749841386127</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" t="n">
-        <v>0.00364234321769412</v>
+        <v>0.00361742212052195</v>
       </c>
       <c r="C7" t="n">
-        <v>0.00163584671660434</v>
+        <v>0.00162451569581588</v>
       </c>
       <c r="D7" t="n">
-        <v>0.00809002453972298</v>
+        <v>0.00803548808215599</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0127641660962478</v>
+        <v>0.0127956136819018</v>
       </c>
       <c r="C8" t="n">
-        <v>0.00833225364576382</v>
+        <v>0.00835263122360129</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0195070348871368</v>
+        <v>0.0195553292882182</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" t="n">
-        <v>0.00976065453590142</v>
+        <v>0.00971548261990875</v>
       </c>
       <c r="C9" t="n">
-        <v>0.00598432332433118</v>
+        <v>0.00595674732102174</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0158819170342182</v>
+        <v>0.0158082789652532</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" t="n">
-        <v>0.00482113293335231</v>
+        <v>0.00484197367483586</v>
       </c>
       <c r="C10" t="n">
-        <v>0.00241069901964735</v>
+        <v>0.00242100990296438</v>
       </c>
       <c r="D10" t="n">
-        <v>0.00961849746077391</v>
+        <v>0.00966041127057929</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" t="n">
-        <v>0.0018327891734277</v>
+        <v>0.00185111449255576</v>
       </c>
       <c r="C11" t="n">
-        <v>0.000590529286787167</v>
+        <v>0.000596426568275955</v>
       </c>
       <c r="D11" t="n">
-        <v>0.00567347917903267</v>
+        <v>0.00573012514957898</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.871503878296706</v>
+        <v>0.871427497063904</v>
       </c>
       <c r="C12" t="n">
-        <v>0.854408992090673</v>
+        <v>0.854323822113845</v>
       </c>
       <c r="D12" t="n">
-        <v>0.88685733324062</v>
+        <v>0.886789155642602</v>
       </c>
     </row>
   </sheetData>
@@ -1222,7 +1619,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
@@ -1251,258 +1648,753 @@
       <c r="J1" t="s">
         <v>14</v>
       </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2"/>
-      <c r="C2" t="n">
-        <v>0.459711565255802</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2"/>
       <c r="D2"/>
       <c r="E2"/>
-      <c r="F2" t="n">
-        <v>0.0761099790356928</v>
-      </c>
-      <c r="G2"/>
-      <c r="H2" t="n">
-        <v>0.309927004551022</v>
-      </c>
+      <c r="F2"/>
+      <c r="G2" t="n">
+        <v>0.0774017191101546</v>
+      </c>
+      <c r="H2"/>
       <c r="I2"/>
-      <c r="J2" t="n">
-        <v>0.154251452000377</v>
-      </c>
+      <c r="J2"/>
+      <c r="K2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0191192273976059</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.379406701348791</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.00928103769840296</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.0366998611008201</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.0932494331785877</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.0182151295798106</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.360588265943902</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
       <c r="I3"/>
-      <c r="J3" t="n">
-        <v>0.0834403445297187</v>
+      <c r="J3"/>
+      <c r="K3" t="n">
+        <v>0.153324987415284</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4"/>
-      <c r="C4" t="n">
-        <v>0.999999999941722</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4"/>
       <c r="D4"/>
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4"/>
-      <c r="I4"/>
+      <c r="I4" t="n">
+        <v>0.306147690908104</v>
+      </c>
       <c r="J4"/>
+      <c r="K4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5"/>
-      <c r="C5" t="n">
-        <v>0.20265531695919</v>
-      </c>
-      <c r="D5"/>
+        <v>29</v>
+      </c>
+      <c r="B5" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5"/>
+      <c r="D5" t="n">
+        <v>0.463125603846068</v>
+      </c>
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5"/>
-      <c r="H5" t="n">
-        <v>0.597465629683135</v>
-      </c>
+      <c r="H5"/>
       <c r="I5"/>
-      <c r="J5" t="n">
-        <v>0.199879053357739</v>
-      </c>
+      <c r="J5"/>
+      <c r="K5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" t="n">
-        <v>0.10845727485072</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.373689313889416</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C6"/>
       <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6" t="n">
-        <v>0.0359082260266671</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.0371055416639959</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.334113955557595</v>
-      </c>
+      <c r="E6" t="n">
+        <v>0.00936468643666993</v>
+      </c>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
       <c r="I6"/>
-      <c r="J6" t="n">
-        <v>0.110725688451475</v>
-      </c>
+      <c r="J6"/>
+      <c r="K6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B7" t="n">
-        <v>0.168220667274258</v>
+        <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>0.332875469764498</v>
+        <v>0.0182917790959609</v>
       </c>
       <c r="D7"/>
       <c r="E7"/>
-      <c r="F7" t="n">
-        <v>0.167491125837844</v>
-      </c>
+      <c r="F7"/>
       <c r="G7"/>
       <c r="H7" t="n">
-        <v>0.331412737603462</v>
+        <v>0.0179556098348943</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
+      <c r="K7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8"/>
-      <c r="C8" t="n">
-        <v>0.192033078025912</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8"/>
       <c r="D8"/>
       <c r="E8"/>
       <c r="F8" t="n">
-        <v>0.189259627641224</v>
+        <v>0.0368319216140686</v>
       </c>
       <c r="G8"/>
-      <c r="H8" t="n">
-        <v>0.428925944507396</v>
-      </c>
+      <c r="H8"/>
       <c r="I8"/>
-      <c r="J8" t="n">
-        <v>0.189781349825487</v>
-      </c>
+      <c r="J8"/>
+      <c r="K8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0614474883176695</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.379903511594133</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C9"/>
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9"/>
-      <c r="G9" t="n">
-        <v>0.0609511689809461</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.373314033630456</v>
-      </c>
+      <c r="G9"/>
+      <c r="H9"/>
       <c r="I9"/>
-      <c r="J9" t="n">
-        <v>0.124383797499537</v>
+      <c r="J9"/>
+      <c r="K9" t="n">
+        <v>0.0827871357014964</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10"/>
-      <c r="C10" t="n">
-        <v>0.750781768365729</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B10" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10"/>
       <c r="D10"/>
       <c r="E10"/>
-      <c r="F10" t="n">
-        <v>0.127994258661491</v>
-      </c>
-      <c r="G10"/>
-      <c r="H10" t="n">
-        <v>0.121223972991958</v>
-      </c>
+      <c r="F10"/>
+      <c r="G10" t="n">
+        <v>0.0933570550027876</v>
+      </c>
+      <c r="H10"/>
       <c r="I10"/>
       <c r="J10"/>
+      <c r="K10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11"/>
-      <c r="C11" t="n">
-        <v>0.330834901041496</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B11" t="n">
+        <v>39</v>
+      </c>
+      <c r="C11"/>
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
-      <c r="H11" t="n">
-        <v>0.669165098958504</v>
-      </c>
-      <c r="I11"/>
+      <c r="H11"/>
+      <c r="I11" t="n">
+        <v>0.362143154760712</v>
+      </c>
       <c r="J11"/>
+      <c r="K11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="n">
+        <v>41</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12" t="n">
+        <v>0.379268658635133</v>
+      </c>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13" t="n">
+        <v>0.999999999941915</v>
+      </c>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14"/>
+      <c r="D14" t="n">
+        <v>0.200344735609395</v>
+      </c>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14" t="n">
+        <v>0.19931178860759</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15" t="n">
+        <v>0.600343475783058</v>
+      </c>
+      <c r="J15"/>
+      <c r="K15"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16" t="n">
+        <v>0.03627557974319</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.0370260930073758</v>
+      </c>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.109796415048989</v>
+      </c>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17" t="n">
+        <v>0.110895353580098</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="n">
         <v>9</v>
       </c>
-      <c r="B12" t="n">
-        <v>0.023793541459921</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.351670150854278</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.00280674876747064</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.0126280324848107</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.0893758834624944</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.0574325855081615</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0.379930000077563</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0.00564048305175319</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.0767225744023766</v>
-      </c>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18" t="n">
+        <v>0.334772344849588</v>
+      </c>
+      <c r="J18"/>
+      <c r="K18"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="n">
+        <v>10</v>
+      </c>
+      <c r="C19"/>
+      <c r="D19" t="n">
+        <v>0.371234214113565</v>
+      </c>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.167926531841217</v>
+      </c>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20" t="n">
+        <v>0.165486680361424</v>
+      </c>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21"/>
+      <c r="D21" t="n">
+        <v>0.333794836453526</v>
+      </c>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21" t="n">
+        <v>0.332791951483967</v>
+      </c>
+      <c r="J21"/>
+      <c r="K21"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="n">
+        <v>4</v>
+      </c>
+      <c r="C22"/>
+      <c r="D22" t="n">
+        <v>0.187939987838969</v>
+      </c>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22" t="n">
+        <v>0.190113289385869</v>
+      </c>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22" t="n">
+        <v>0.19121126328733</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="n">
+        <v>9</v>
+      </c>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23" t="n">
+        <v>0.43073545948785</v>
+      </c>
+      <c r="J23"/>
+      <c r="K23"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.0634187029686192</v>
+      </c>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24" t="n">
+        <v>0.0612966409947904</v>
+      </c>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25" t="n">
+        <v>0.123665642506358</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" t="n">
+        <v>6</v>
+      </c>
+      <c r="C26"/>
+      <c r="D26" t="n">
+        <v>0.374218065385169</v>
+      </c>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26" t="n">
+        <v>0.37740094816547</v>
+      </c>
+      <c r="J26"/>
+      <c r="K26"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27" t="n">
+        <v>0.123922567958281</v>
+      </c>
+      <c r="H27"/>
+      <c r="I27" t="n">
+        <v>0.122863419142676</v>
+      </c>
+      <c r="J27"/>
+      <c r="K27"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" t="n">
+        <v>6</v>
+      </c>
+      <c r="C28"/>
+      <c r="D28" t="n">
+        <v>0.753214012915785</v>
+      </c>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29"/>
+      <c r="D29" t="n">
+        <v>0.337329216278065</v>
+      </c>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" t="n">
+        <v>2</v>
+      </c>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30" t="n">
+        <v>0.662670783721935</v>
+      </c>
+      <c r="J30"/>
+      <c r="K30"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" t="n">
+        <v>4</v>
+      </c>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31" t="n">
+        <v>0.00279789604551283</v>
+      </c>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" t="n">
+        <v>8</v>
+      </c>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32" t="n">
+        <v>0.00555613052822659</v>
+      </c>
+      <c r="K32"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" t="n">
+        <v>18</v>
+      </c>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33" t="n">
+        <v>0.0126053011259347</v>
+      </c>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="n">
+        <v>34</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.0238346296368123</v>
+      </c>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" t="n">
+        <v>82</v>
+      </c>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35" t="n">
+        <v>0.0573623325048403</v>
+      </c>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" t="n">
+        <v>110</v>
+      </c>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36" t="n">
+        <v>0.0769392035900961</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" t="n">
+        <v>128</v>
+      </c>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37" t="n">
+        <v>0.0893358677058636</v>
+      </c>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" t="n">
+        <v>503</v>
+      </c>
+      <c r="C38"/>
+      <c r="D38" t="n">
+        <v>0.351769347945508</v>
+      </c>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" t="n">
+        <v>544</v>
+      </c>
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39" t="n">
+        <v>0.379799290987512</v>
+      </c>
+      <c r="J39"/>
+      <c r="K39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1520,10 +2412,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>
@@ -1537,178 +2429,448 @@
       <c r="F1" t="s">
         <v>19</v>
       </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" t="n">
-        <v>0.539338172498516</v>
+        <v>6</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
-      <c r="E2" t="n">
-        <v>0.460661827501484</v>
-      </c>
-      <c r="F2"/>
+      <c r="E2"/>
+      <c r="F2" t="n">
+        <v>0.462444208317141</v>
+      </c>
+      <c r="G2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
       <c r="B3" t="n">
-        <v>0.60241655815913</v>
+        <v>7</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0274618535762502</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.056036544438785</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.305014107845379</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.00907093603041663</v>
-      </c>
+        <v>0.537555791682859</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>30</v>
       </c>
       <c r="B4" t="n">
-        <v>0.498854512930488</v>
+        <v>1</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
-      <c r="E4" t="n">
-        <v>0.501145487069512</v>
-      </c>
+      <c r="E4"/>
       <c r="F4"/>
+      <c r="G4" t="n">
+        <v>0.00899472349940583</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" t="n">
-        <v>0.802743755293758</v>
+        <v>3</v>
       </c>
       <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5" t="n">
-        <v>0.197256244706242</v>
-      </c>
+      <c r="D5" t="n">
+        <v>0.0277780535808537</v>
+      </c>
+      <c r="E5"/>
       <c r="F5"/>
+      <c r="G5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" t="n">
-        <v>0.369588431218004</v>
+        <v>6</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
       <c r="E6" t="n">
-        <v>0.555044262022936</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.0753673064961356</v>
-      </c>
+        <v>0.0560620779676171</v>
+      </c>
+      <c r="F6"/>
+      <c r="G6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="n">
         <v>33</v>
       </c>
-      <c r="B7" t="n">
-        <v>0.498903863277399</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.168220667274258</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.332875469764498</v>
-      </c>
+      <c r="C7"/>
+      <c r="D7"/>
       <c r="E7"/>
-      <c r="F7"/>
+      <c r="F7" t="n">
+        <v>0.30438741292904</v>
+      </c>
+      <c r="G7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B8" t="n">
-        <v>0.379238529339389</v>
+        <v>65</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0495498689267511</v>
+        <v>0.602777732073283</v>
       </c>
       <c r="D8"/>
-      <c r="E8" t="n">
-        <v>0.571211602051116</v>
-      </c>
+      <c r="E8"/>
       <c r="F8"/>
+      <c r="G8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B9" t="n">
-        <v>0.376114317176781</v>
-      </c>
-      <c r="C9"/>
+        <v>2</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.495676723193105</v>
+      </c>
       <c r="D9"/>
-      <c r="E9" t="n">
-        <v>0.623885682823219</v>
-      </c>
-      <c r="F9"/>
+      <c r="E9"/>
+      <c r="F9" t="n">
+        <v>0.504323276806895</v>
+      </c>
+      <c r="G9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B10" t="n">
-        <v>0.506225221731354</v>
+        <v>1</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
-      <c r="E10" t="n">
-        <v>0.493774778268647</v>
-      </c>
-      <c r="F10"/>
+      <c r="E10"/>
+      <c r="F10" t="n">
+        <v>0.204769730990452</v>
+      </c>
+      <c r="G10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B11" t="n">
-        <v>0.33487034793763</v>
-      </c>
-      <c r="C11"/>
+        <v>4</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.795230269009548</v>
+      </c>
       <c r="D11"/>
-      <c r="E11" t="n">
-        <v>0.66512965206237</v>
-      </c>
+      <c r="E11"/>
       <c r="F11"/>
+      <c r="G11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B12" t="n">
-        <v>0.600545267246648</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.00909141546023589</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.0377252370539632</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.33724064569999</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.0153974345448258</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12" t="n">
+        <v>0.0737103820044227</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="n">
+        <v>10</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.370225924287712</v>
+      </c>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="n">
+        <v>15</v>
+      </c>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14" t="n">
+        <v>0.556063693424929</v>
+      </c>
+      <c r="G14"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15"/>
+      <c r="D15" t="n">
+        <v>0.167926531841217</v>
+      </c>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16" t="n">
+        <v>0.333794836453526</v>
+      </c>
+      <c r="F16"/>
+      <c r="G16"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.49827863185786</v>
+      </c>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18"/>
+      <c r="D18" t="n">
+        <v>0.0473017870287397</v>
+      </c>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="n">
+        <v>8</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.377604433227111</v>
+      </c>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="n">
+        <v>12</v>
+      </c>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20" t="n">
+        <v>0.575093780381481</v>
+      </c>
+      <c r="G20"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="n">
+        <v>6</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.378193814315582</v>
+      </c>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="n">
+        <v>10</v>
+      </c>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22" t="n">
+        <v>0.621806185684418</v>
+      </c>
+      <c r="G22"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" t="n">
+        <v>4</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.497109013771201</v>
+      </c>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23" t="n">
+        <v>0.502890986228799</v>
+      </c>
+      <c r="G23"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.331320321077042</v>
+      </c>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25" t="n">
+        <v>0.668679678922958</v>
+      </c>
+      <c r="G25"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="n">
+        <v>13</v>
+      </c>
+      <c r="C26"/>
+      <c r="D26" t="n">
+        <v>0.00896737318782599</v>
+      </c>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="n">
+        <v>22</v>
+      </c>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27" t="n">
+        <v>0.0154411482554869</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" t="n">
+        <v>54</v>
+      </c>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28" t="n">
+        <v>0.0377978901201288</v>
+      </c>
+      <c r="F28"/>
+      <c r="G28"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="n">
+        <v>483</v>
+      </c>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29" t="n">
+        <v>0.337579574555633</v>
+      </c>
+      <c r="G29"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="n">
+        <v>859</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.600214013887846</v>
+      </c>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>